<commit_message>
Second method, changed to use actual magnetic field values instead of current/voltage
</commit_message>
<xml_diff>
--- a/faraday/data/hysteresis.xlsx
+++ b/faraday/data/hysteresis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackson\physics_387\faraday\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C506BC-320E-42F1-8691-E4CDC1D26F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DB82E5-86AD-48E2-B940-CF2B8BEC4433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F18BD550-01FC-4343-9ECC-2B973BA55216}"/>
   </bookViews>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DFF23A-18AC-40F0-89AD-EBBDE2D5C48B}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>